<commit_message>
Adicionando autodeclaração dos candidatos e criando base de dados do Brasil
</commit_message>
<xml_diff>
--- a/2018/Centro-Oeste/MS/resultado.xlsx
+++ b/2018/Centro-Oeste/MS/resultado.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N131"/>
+  <dimension ref="A1:R131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,12 +496,32 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
+          <t>SG_PARTIDO_x</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>DS_ESTADO_CIVIL</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>DS_GRAU_INSTRUCAO</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>SG_PARTIDO_y</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
           <t>SQ_CANDIDATO</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>SG_PARTIDO</t>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>DS_COR_RACA</t>
         </is>
       </c>
     </row>
@@ -564,12 +584,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M2" t="n">
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>NOVO</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>NOVO</t>
+        </is>
+      </c>
+      <c r="Q2" t="n">
         <v>120000600192</v>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>NOVO</t>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -632,12 +672,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M3" t="n">
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>NOVO</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>NOVO</t>
+        </is>
+      </c>
+      <c r="Q3" t="n">
         <v>120000600193</v>
       </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>NOVO</t>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -700,12 +760,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M4" t="n">
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>NOVO</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>NOVO</t>
+        </is>
+      </c>
+      <c r="Q4" t="n">
         <v>120000600194</v>
       </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>NOVO</t>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -768,12 +848,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M5" t="n">
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>NOVO</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>NOVO</t>
+        </is>
+      </c>
+      <c r="Q5" t="n">
         <v>120000600195</v>
       </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>NOVO</t>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -836,12 +936,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M6" t="n">
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>NOVO</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>NOVO</t>
+        </is>
+      </c>
+      <c r="Q6" t="n">
         <v>120000600196</v>
       </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>NOVO</t>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -904,12 +1024,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M7" t="n">
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
+      <c r="Q7" t="n">
         <v>120000602218</v>
       </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>PDT</t>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -972,12 +1112,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M8" t="n">
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
+      <c r="Q8" t="n">
         <v>120000602219</v>
       </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>PDT</t>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -1040,12 +1200,32 @@
           <t>ENSINO FUNDAMENTAL INCOMPLETO</t>
         </is>
       </c>
-      <c r="M9" t="n">
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
+      <c r="Q9" t="n">
         <v>120000602220</v>
       </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>PDT</t>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -1108,12 +1288,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M10" t="n">
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
+      <c r="Q10" t="n">
         <v>120000602221</v>
       </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>PDT</t>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -1176,12 +1376,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M11" t="n">
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
+      <c r="Q11" t="n">
         <v>120000602222</v>
       </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>PDT</t>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -1244,12 +1464,32 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
-      <c r="M12" t="n">
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
+      <c r="Q12" t="n">
         <v>120000602223</v>
       </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>PDT</t>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -1312,12 +1552,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M13" t="n">
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
+      <c r="Q13" t="n">
         <v>120000602224</v>
       </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>PDT</t>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -1380,12 +1640,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M14" t="n">
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
+      <c r="Q14" t="n">
         <v>120000602225</v>
       </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>PDT</t>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -1448,12 +1728,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M15" t="n">
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>PRB</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>PRB</t>
+        </is>
+      </c>
+      <c r="Q15" t="n">
         <v>120000602226</v>
       </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>PRB</t>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -1516,12 +1816,32 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
-      <c r="M16" t="n">
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>PRB</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>PRB</t>
+        </is>
+      </c>
+      <c r="Q16" t="n">
         <v>120000602227</v>
       </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>PRB</t>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -1584,12 +1904,32 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
-      <c r="M17" t="n">
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>PRB</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>PRB</t>
+        </is>
+      </c>
+      <c r="Q17" t="n">
         <v>120000602228</v>
       </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>PRB</t>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -1652,12 +1992,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M18" t="n">
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>PODE</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>PODE</t>
+        </is>
+      </c>
+      <c r="Q18" t="n">
         <v>120000602229</v>
       </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>PODE</t>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -1720,12 +2080,32 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
-      <c r="M19" t="n">
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>PODE</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>PODE</t>
+        </is>
+      </c>
+      <c r="Q19" t="n">
         <v>120000602230</v>
       </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>PODE</t>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -1788,12 +2168,32 @@
           <t>LÊ E ESCREVE</t>
         </is>
       </c>
-      <c r="M20" t="n">
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>PODE</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>LÊ E ESCREVE</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>PODE</t>
+        </is>
+      </c>
+      <c r="Q20" t="n">
         <v>120000602231</v>
       </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>PODE</t>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -1856,12 +2256,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M21" t="n">
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>PODE</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>PODE</t>
+        </is>
+      </c>
+      <c r="Q21" t="n">
         <v>120000602232</v>
       </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>PODE</t>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -1924,12 +2344,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M22" t="n">
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>PODE</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>PODE</t>
+        </is>
+      </c>
+      <c r="Q22" t="n">
         <v>120000602233</v>
       </c>
-      <c r="N22" t="inlineStr">
-        <is>
-          <t>PODE</t>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -1992,12 +2432,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M23" t="n">
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
+      <c r="Q23" t="n">
         <v>120000605500</v>
       </c>
-      <c r="N23" t="inlineStr">
-        <is>
-          <t>PV</t>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -2060,12 +2520,32 @@
           <t>ENSINO FUNDAMENTAL INCOMPLETO</t>
         </is>
       </c>
-      <c r="M24" t="n">
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
+      <c r="Q24" t="n">
         <v>120000605503</v>
       </c>
-      <c r="N24" t="inlineStr">
-        <is>
-          <t>PV</t>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -2128,12 +2608,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M25" t="n">
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
+      <c r="Q25" t="n">
         <v>120000605507</v>
       </c>
-      <c r="N25" t="inlineStr">
-        <is>
-          <t>PV</t>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -2196,12 +2696,32 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
-      <c r="M26" t="n">
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
+      <c r="Q26" t="n">
         <v>120000605511</v>
       </c>
-      <c r="N26" t="inlineStr">
-        <is>
-          <t>PV</t>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -2264,12 +2784,32 @@
           <t>ENSINO FUNDAMENTAL COMPLETO</t>
         </is>
       </c>
-      <c r="M27" t="n">
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL COMPLETO</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
+      <c r="Q27" t="n">
         <v>120000605525</v>
       </c>
-      <c r="N27" t="inlineStr">
-        <is>
-          <t>PV</t>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -2332,12 +2872,32 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
-      <c r="M28" t="n">
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>PC do B</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>PC do B</t>
+        </is>
+      </c>
+      <c r="Q28" t="n">
         <v>120000605527</v>
       </c>
-      <c r="N28" t="inlineStr">
-        <is>
-          <t>PC do B</t>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -2400,12 +2960,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M29" t="n">
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>REDE</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>REDE</t>
+        </is>
+      </c>
+      <c r="Q29" t="n">
         <v>120000605529</v>
       </c>
-      <c r="N29" t="inlineStr">
-        <is>
-          <t>REDE</t>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -2468,12 +3048,32 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
-      <c r="M30" t="n">
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
+      <c r="Q30" t="n">
         <v>120000605530</v>
       </c>
-      <c r="N30" t="inlineStr">
-        <is>
-          <t>PV</t>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -2536,12 +3136,32 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
-      <c r="M31" t="n">
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>REDE</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>REDE</t>
+        </is>
+      </c>
+      <c r="Q31" t="n">
         <v>120000605531</v>
       </c>
-      <c r="N31" t="inlineStr">
-        <is>
-          <t>REDE</t>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -2604,12 +3224,32 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
-      <c r="M32" t="n">
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>REDE</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>REDE</t>
+        </is>
+      </c>
+      <c r="Q32" t="n">
         <v>120000605532</v>
       </c>
-      <c r="N32" t="inlineStr">
-        <is>
-          <t>REDE</t>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -2672,12 +3312,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M33" t="n">
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>PC do B</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>PC do B</t>
+        </is>
+      </c>
+      <c r="Q33" t="n">
         <v>120000605534</v>
       </c>
-      <c r="N33" t="inlineStr">
-        <is>
-          <t>PC do B</t>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -2740,12 +3400,32 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
-      <c r="M34" t="n">
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>PC do B</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>PC do B</t>
+        </is>
+      </c>
+      <c r="Q34" t="n">
         <v>120000605535</v>
       </c>
-      <c r="N34" t="inlineStr">
-        <is>
-          <t>PC do B</t>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -2808,12 +3488,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M35" t="n">
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
+      <c r="Q35" t="n">
         <v>120000605537</v>
       </c>
-      <c r="N35" t="inlineStr">
-        <is>
-          <t>PV</t>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -2876,12 +3576,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M36" t="n">
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>REDE</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>REDE</t>
+        </is>
+      </c>
+      <c r="Q36" t="n">
         <v>120000605538</v>
       </c>
-      <c r="N36" t="inlineStr">
-        <is>
-          <t>REDE</t>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>PRETA</t>
         </is>
       </c>
     </row>
@@ -2944,12 +3664,32 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
-      <c r="M37" t="n">
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
+      <c r="Q37" t="n">
         <v>120000612723</v>
       </c>
-      <c r="N37" t="inlineStr">
-        <is>
-          <t>PSOL</t>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>PRETA</t>
         </is>
       </c>
     </row>
@@ -3012,12 +3752,32 @@
           <t>ENSINO FUNDAMENTAL COMPLETO</t>
         </is>
       </c>
-      <c r="M38" t="n">
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL COMPLETO</t>
+        </is>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
+      <c r="Q38" t="n">
         <v>120000612724</v>
       </c>
-      <c r="N38" t="inlineStr">
-        <is>
-          <t>PSOL</t>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -3080,12 +3840,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M39" t="n">
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
+      <c r="Q39" t="n">
         <v>120000612725</v>
       </c>
-      <c r="N39" t="inlineStr">
-        <is>
-          <t>PSOL</t>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -3148,12 +3928,32 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
-      <c r="M40" t="n">
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
+      <c r="Q40" t="n">
         <v>120000612726</v>
       </c>
-      <c r="N40" t="inlineStr">
-        <is>
-          <t>PSOL</t>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -3216,12 +4016,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M41" t="n">
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
+      <c r="Q41" t="n">
         <v>120000612727</v>
       </c>
-      <c r="N41" t="inlineStr">
-        <is>
-          <t>PSOL</t>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>PRETA</t>
         </is>
       </c>
     </row>
@@ -3284,12 +4104,32 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
-      <c r="M42" t="n">
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
+      <c r="Q42" t="n">
         <v>120000612728</v>
       </c>
-      <c r="N42" t="inlineStr">
-        <is>
-          <t>PSOL</t>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -3352,12 +4192,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M43" t="n">
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
+      <c r="Q43" t="n">
         <v>120000613453</v>
       </c>
-      <c r="N43" t="inlineStr">
-        <is>
-          <t>PSDB</t>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -3420,12 +4280,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M44" t="n">
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>VIÚVO(A)</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
+      <c r="Q44" t="n">
         <v>120000613454</v>
       </c>
-      <c r="N44" t="inlineStr">
-        <is>
-          <t>PSDB</t>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -3488,12 +4368,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M45" t="n">
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
+      <c r="Q45" t="n">
         <v>120000613455</v>
       </c>
-      <c r="N45" t="inlineStr">
-        <is>
-          <t>PSDB</t>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -3556,12 +4456,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M46" t="n">
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
+      <c r="Q46" t="n">
         <v>120000613456</v>
       </c>
-      <c r="N46" t="inlineStr">
-        <is>
-          <t>PSDB</t>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -3624,12 +4544,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M47" t="n">
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
+      <c r="Q47" t="n">
         <v>120000613457</v>
       </c>
-      <c r="N47" t="inlineStr">
-        <is>
-          <t>PSDB</t>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -3692,12 +4632,32 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
-      <c r="M48" t="n">
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>PMB</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>PMB</t>
+        </is>
+      </c>
+      <c r="Q48" t="n">
         <v>120000613458</v>
       </c>
-      <c r="N48" t="inlineStr">
-        <is>
-          <t>PMB</t>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -3760,12 +4720,32 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
-      <c r="M49" t="n">
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>PSD</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>PSD</t>
+        </is>
+      </c>
+      <c r="Q49" t="n">
         <v>120000613459</v>
       </c>
-      <c r="N49" t="inlineStr">
-        <is>
-          <t>PSD</t>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>PRETA</t>
         </is>
       </c>
     </row>
@@ -3828,12 +4808,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M50" t="n">
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>DEM</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t>DEM</t>
+        </is>
+      </c>
+      <c r="Q50" t="n">
         <v>120000613460</v>
       </c>
-      <c r="N50" t="inlineStr">
-        <is>
-          <t>DEM</t>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -3896,12 +4896,32 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
-      <c r="M51" t="n">
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>DEM</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t>DEM</t>
+        </is>
+      </c>
+      <c r="Q51" t="n">
         <v>120000613461</v>
       </c>
-      <c r="N51" t="inlineStr">
-        <is>
-          <t>DEM</t>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -3964,12 +4984,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M52" t="n">
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>DEM</t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t>DEM</t>
+        </is>
+      </c>
+      <c r="Q52" t="n">
         <v>120000613462</v>
       </c>
-      <c r="N52" t="inlineStr">
-        <is>
-          <t>DEM</t>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -4032,12 +5072,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M53" t="n">
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>PSD</t>
+        </is>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P53" t="inlineStr">
+        <is>
+          <t>PSD</t>
+        </is>
+      </c>
+      <c r="Q53" t="n">
         <v>120000613463</v>
       </c>
-      <c r="N53" t="inlineStr">
-        <is>
-          <t>PSD</t>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -4100,12 +5160,32 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
-      <c r="M54" t="n">
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>DEM</t>
+        </is>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t>DEM</t>
+        </is>
+      </c>
+      <c r="Q54" t="n">
         <v>120000613464</v>
       </c>
-      <c r="N54" t="inlineStr">
-        <is>
-          <t>DEM</t>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -4168,12 +5248,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M55" t="n">
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>DEM</t>
+        </is>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P55" t="inlineStr">
+        <is>
+          <t>DEM</t>
+        </is>
+      </c>
+      <c r="Q55" t="n">
         <v>120000613465</v>
       </c>
-      <c r="N55" t="inlineStr">
-        <is>
-          <t>DEM</t>
+      <c r="R55" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -4236,12 +5336,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M56" t="n">
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>PP</t>
+        </is>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P56" t="inlineStr">
+        <is>
+          <t>PP</t>
+        </is>
+      </c>
+      <c r="Q56" t="n">
         <v>120000613466</v>
       </c>
-      <c r="N56" t="inlineStr">
-        <is>
-          <t>PP</t>
+      <c r="R56" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -4304,12 +5424,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M57" t="n">
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>PATRIOTA</t>
+        </is>
+      </c>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P57" t="inlineStr">
+        <is>
+          <t>PATRIOTA</t>
+        </is>
+      </c>
+      <c r="Q57" t="n">
         <v>120000613467</v>
       </c>
-      <c r="N57" t="inlineStr">
-        <is>
-          <t>PATRIOTA</t>
+      <c r="R57" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -4372,12 +5512,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M58" t="n">
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>PATRIOTA</t>
+        </is>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P58" t="inlineStr">
+        <is>
+          <t>PATRIOTA</t>
+        </is>
+      </c>
+      <c r="Q58" t="n">
         <v>120000613468</v>
       </c>
-      <c r="N58" t="inlineStr">
-        <is>
-          <t>PATRIOTA</t>
+      <c r="R58" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -4440,12 +5600,32 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
-      <c r="M59" t="n">
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>PTB</t>
+        </is>
+      </c>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="P59" t="inlineStr">
+        <is>
+          <t>PTB</t>
+        </is>
+      </c>
+      <c r="Q59" t="n">
         <v>120000615481</v>
       </c>
-      <c r="N59" t="inlineStr">
-        <is>
-          <t>PTB</t>
+      <c r="R59" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -4508,12 +5688,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M60" t="n">
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>PSL</t>
+        </is>
+      </c>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P60" t="inlineStr">
+        <is>
+          <t>PSL</t>
+        </is>
+      </c>
+      <c r="Q60" t="n">
         <v>120000615482</v>
       </c>
-      <c r="N60" t="inlineStr">
-        <is>
-          <t>PSL</t>
+      <c r="R60" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -4576,12 +5776,32 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
-      <c r="M61" t="n">
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>PSL</t>
+        </is>
+      </c>
+      <c r="N61" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="P61" t="inlineStr">
+        <is>
+          <t>PSL</t>
+        </is>
+      </c>
+      <c r="Q61" t="n">
         <v>120000615483</v>
       </c>
-      <c r="N61" t="inlineStr">
-        <is>
-          <t>PSL</t>
+      <c r="R61" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -4644,12 +5864,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M62" t="n">
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>PSL</t>
+        </is>
+      </c>
+      <c r="N62" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P62" t="inlineStr">
+        <is>
+          <t>PSL</t>
+        </is>
+      </c>
+      <c r="Q62" t="n">
         <v>120000615484</v>
       </c>
-      <c r="N62" t="inlineStr">
-        <is>
-          <t>PSL</t>
+      <c r="R62" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -4712,12 +5952,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M63" t="n">
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>PSL</t>
+        </is>
+      </c>
+      <c r="N63" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P63" t="inlineStr">
+        <is>
+          <t>PSL</t>
+        </is>
+      </c>
+      <c r="Q63" t="n">
         <v>120000615485</v>
       </c>
-      <c r="N63" t="inlineStr">
-        <is>
-          <t>PSL</t>
+      <c r="R63" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -4780,12 +6040,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M64" t="n">
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>PSB</t>
+        </is>
+      </c>
+      <c r="N64" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P64" t="inlineStr">
+        <is>
+          <t>PSB</t>
+        </is>
+      </c>
+      <c r="Q64" t="n">
         <v>120000615486</v>
       </c>
-      <c r="N64" t="inlineStr">
-        <is>
-          <t>PSB</t>
+      <c r="R64" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -4848,12 +6128,32 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
-      <c r="M65" t="n">
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>PPS</t>
+        </is>
+      </c>
+      <c r="N65" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="P65" t="inlineStr">
+        <is>
+          <t>PPS</t>
+        </is>
+      </c>
+      <c r="Q65" t="n">
         <v>120000615487</v>
       </c>
-      <c r="N65" t="inlineStr">
-        <is>
-          <t>PPS</t>
+      <c r="R65" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -4916,12 +6216,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M66" t="n">
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>PROS</t>
+        </is>
+      </c>
+      <c r="N66" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P66" t="inlineStr">
+        <is>
+          <t>PROS</t>
+        </is>
+      </c>
+      <c r="Q66" t="n">
         <v>120000615488</v>
       </c>
-      <c r="N66" t="inlineStr">
-        <is>
-          <t>PROS</t>
+      <c r="R66" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -4984,12 +6304,32 @@
           <t>LÊ E ESCREVE</t>
         </is>
       </c>
-      <c r="M67" t="n">
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>PROS</t>
+        </is>
+      </c>
+      <c r="N67" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>LÊ E ESCREVE</t>
+        </is>
+      </c>
+      <c r="P67" t="inlineStr">
+        <is>
+          <t>PROS</t>
+        </is>
+      </c>
+      <c r="Q67" t="n">
         <v>120000615489</v>
       </c>
-      <c r="N67" t="inlineStr">
-        <is>
-          <t>PROS</t>
+      <c r="R67" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -5052,12 +6392,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M68" t="n">
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>PROS</t>
+        </is>
+      </c>
+      <c r="N68" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P68" t="inlineStr">
+        <is>
+          <t>PROS</t>
+        </is>
+      </c>
+      <c r="Q68" t="n">
         <v>120000615490</v>
       </c>
-      <c r="N68" t="inlineStr">
-        <is>
-          <t>PROS</t>
+      <c r="R68" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -5120,12 +6480,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M69" t="n">
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>PROS</t>
+        </is>
+      </c>
+      <c r="N69" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P69" t="inlineStr">
+        <is>
+          <t>PROS</t>
+        </is>
+      </c>
+      <c r="Q69" t="n">
         <v>120000615491</v>
       </c>
-      <c r="N69" t="inlineStr">
-        <is>
-          <t>PROS</t>
+      <c r="R69" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -5188,12 +6568,32 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
-      <c r="M70" t="n">
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>SOLIDARIEDADE</t>
+        </is>
+      </c>
+      <c r="N70" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="P70" t="inlineStr">
+        <is>
+          <t>SOLIDARIEDADE</t>
+        </is>
+      </c>
+      <c r="Q70" t="n">
         <v>120000615492</v>
       </c>
-      <c r="N70" t="inlineStr">
-        <is>
-          <t>SOLIDARIEDADE</t>
+      <c r="R70" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -5256,12 +6656,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M71" t="n">
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>SOLIDARIEDADE</t>
+        </is>
+      </c>
+      <c r="N71" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P71" t="inlineStr">
+        <is>
+          <t>SOLIDARIEDADE</t>
+        </is>
+      </c>
+      <c r="Q71" t="n">
         <v>120000615493</v>
       </c>
-      <c r="N71" t="inlineStr">
-        <is>
-          <t>SOLIDARIEDADE</t>
+      <c r="R71" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -5324,12 +6744,32 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
-      <c r="M72" t="n">
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>PMN</t>
+        </is>
+      </c>
+      <c r="N72" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="P72" t="inlineStr">
+        <is>
+          <t>PMN</t>
+        </is>
+      </c>
+      <c r="Q72" t="n">
         <v>120000615494</v>
       </c>
-      <c r="N72" t="inlineStr">
-        <is>
-          <t>PMN</t>
+      <c r="R72" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -5392,12 +6832,32 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
-      <c r="M73" t="n">
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>AVANTE</t>
+        </is>
+      </c>
+      <c r="N73" t="inlineStr">
+        <is>
+          <t>VIÚVO(A)</t>
+        </is>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="P73" t="inlineStr">
+        <is>
+          <t>AVANTE</t>
+        </is>
+      </c>
+      <c r="Q73" t="n">
         <v>120000615495</v>
       </c>
-      <c r="N73" t="inlineStr">
-        <is>
-          <t>AVANTE</t>
+      <c r="R73" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -5460,12 +6920,32 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
-      <c r="M74" t="n">
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>PPS</t>
+        </is>
+      </c>
+      <c r="N74" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="P74" t="inlineStr">
+        <is>
+          <t>PPS</t>
+        </is>
+      </c>
+      <c r="Q74" t="n">
         <v>120000615496</v>
       </c>
-      <c r="N74" t="inlineStr">
-        <is>
-          <t>PPS</t>
+      <c r="R74" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -5528,12 +7008,32 @@
           <t>LÊ E ESCREVE</t>
         </is>
       </c>
-      <c r="M75" t="n">
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>PCO</t>
+        </is>
+      </c>
+      <c r="N75" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>LÊ E ESCREVE</t>
+        </is>
+      </c>
+      <c r="P75" t="inlineStr">
+        <is>
+          <t>PCO</t>
+        </is>
+      </c>
+      <c r="Q75" t="n">
         <v>120000619283</v>
       </c>
-      <c r="N75" t="inlineStr">
-        <is>
-          <t>PCO</t>
+      <c r="R75" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -5596,12 +7096,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M76" t="n">
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="N76" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P76" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="Q76" t="n">
         <v>120000620224</v>
       </c>
-      <c r="N76" t="inlineStr">
-        <is>
-          <t>PT</t>
+      <c r="R76" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -5664,12 +7184,32 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
-      <c r="M77" t="n">
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="N77" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="P77" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="Q77" t="n">
         <v>120000620240</v>
       </c>
-      <c r="N77" t="inlineStr">
-        <is>
-          <t>PT</t>
+      <c r="R77" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -5732,12 +7272,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M78" t="n">
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="N78" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P78" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="Q78" t="n">
         <v>120000620241</v>
       </c>
-      <c r="N78" t="inlineStr">
-        <is>
-          <t>PT</t>
+      <c r="R78" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -5800,12 +7360,32 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
-      <c r="M79" t="n">
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="N79" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="P79" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="Q79" t="n">
         <v>120000620242</v>
       </c>
-      <c r="N79" t="inlineStr">
-        <is>
-          <t>PT</t>
+      <c r="R79" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -5868,12 +7448,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M80" t="n">
+      <c r="M80" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="N80" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P80" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="Q80" t="n">
         <v>120000620243</v>
       </c>
-      <c r="N80" t="inlineStr">
-        <is>
-          <t>PT</t>
+      <c r="R80" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -5936,12 +7536,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M81" t="n">
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="N81" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P81" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="Q81" t="n">
         <v>120000620247</v>
       </c>
-      <c r="N81" t="inlineStr">
-        <is>
-          <t>PT</t>
+      <c r="R81" t="inlineStr">
+        <is>
+          <t>PRETA</t>
         </is>
       </c>
     </row>
@@ -6004,12 +7624,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M82" t="n">
+      <c r="M82" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="N82" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P82" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="Q82" t="n">
         <v>120000620248</v>
       </c>
-      <c r="N82" t="inlineStr">
-        <is>
-          <t>PT</t>
+      <c r="R82" t="inlineStr">
+        <is>
+          <t>PRETA</t>
         </is>
       </c>
     </row>
@@ -6072,12 +7712,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M83" t="n">
+      <c r="M83" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="N83" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P83" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="Q83" t="n">
         <v>120000620249</v>
       </c>
-      <c r="N83" t="inlineStr">
-        <is>
-          <t>PT</t>
+      <c r="R83" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -6140,12 +7800,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M84" t="n">
+      <c r="M84" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="N84" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P84" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="Q84" t="n">
         <v>120000620250</v>
       </c>
-      <c r="N84" t="inlineStr">
-        <is>
-          <t>PT</t>
+      <c r="R84" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -6208,12 +7888,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M85" t="n">
+      <c r="M85" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="N85" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P85" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="Q85" t="n">
         <v>120000620252</v>
       </c>
-      <c r="N85" t="inlineStr">
-        <is>
-          <t>PT</t>
+      <c r="R85" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -6276,12 +7976,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M86" t="n">
+      <c r="M86" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="N86" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P86" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="Q86" t="n">
         <v>120000620258</v>
       </c>
-      <c r="N86" t="inlineStr">
-        <is>
-          <t>PT</t>
+      <c r="R86" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -6344,12 +8064,32 @@
           <t>ENSINO FUNDAMENTAL INCOMPLETO</t>
         </is>
       </c>
-      <c r="M87" t="n">
+      <c r="M87" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="N87" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="P87" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="Q87" t="n">
         <v>120000620259</v>
       </c>
-      <c r="N87" t="inlineStr">
-        <is>
-          <t>PT</t>
+      <c r="R87" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -6412,12 +8152,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M88" t="n">
+      <c r="M88" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="N88" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P88" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="Q88" t="n">
         <v>120000620265</v>
       </c>
-      <c r="N88" t="inlineStr">
-        <is>
-          <t>PT</t>
+      <c r="R88" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -6480,12 +8240,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M89" t="n">
+      <c r="M89" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="N89" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P89" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="Q89" t="n">
         <v>120000620269</v>
       </c>
-      <c r="N89" t="inlineStr">
-        <is>
-          <t>PT</t>
+      <c r="R89" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -6548,12 +8328,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M90" t="n">
+      <c r="M90" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="N90" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P90" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="Q90" t="n">
         <v>120000620271</v>
       </c>
-      <c r="N90" t="inlineStr">
-        <is>
-          <t>PT</t>
+      <c r="R90" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -6616,12 +8416,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M91" t="n">
+      <c r="M91" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="N91" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P91" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="Q91" t="n">
         <v>120000620272</v>
       </c>
-      <c r="N91" t="inlineStr">
-        <is>
-          <t>PT</t>
+      <c r="R91" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -6684,12 +8504,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M92" t="n">
+      <c r="M92" t="inlineStr">
+        <is>
+          <t>PHS</t>
+        </is>
+      </c>
+      <c r="N92" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P92" t="inlineStr">
+        <is>
+          <t>PHS</t>
+        </is>
+      </c>
+      <c r="Q92" t="n">
         <v>120000624918</v>
       </c>
-      <c r="N92" t="inlineStr">
-        <is>
-          <t>PHS</t>
+      <c r="R92" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -6752,12 +8592,32 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
-      <c r="M93" t="n">
+      <c r="M93" t="inlineStr">
+        <is>
+          <t>PHS</t>
+        </is>
+      </c>
+      <c r="N93" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="P93" t="inlineStr">
+        <is>
+          <t>PHS</t>
+        </is>
+      </c>
+      <c r="Q93" t="n">
         <v>120000624919</v>
       </c>
-      <c r="N93" t="inlineStr">
-        <is>
-          <t>PHS</t>
+      <c r="R93" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -6820,12 +8680,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M94" t="n">
+      <c r="M94" t="inlineStr">
+        <is>
+          <t>PHS</t>
+        </is>
+      </c>
+      <c r="N94" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P94" t="inlineStr">
+        <is>
+          <t>PHS</t>
+        </is>
+      </c>
+      <c r="Q94" t="n">
         <v>120000624920</v>
       </c>
-      <c r="N94" t="inlineStr">
-        <is>
-          <t>PHS</t>
+      <c r="R94" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -6888,12 +8768,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M95" t="n">
+      <c r="M95" t="inlineStr">
+        <is>
+          <t>PHS</t>
+        </is>
+      </c>
+      <c r="N95" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P95" t="inlineStr">
+        <is>
+          <t>PHS</t>
+        </is>
+      </c>
+      <c r="Q95" t="n">
         <v>120000624921</v>
       </c>
-      <c r="N95" t="inlineStr">
-        <is>
-          <t>PHS</t>
+      <c r="R95" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -6956,12 +8856,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M96" t="n">
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>PR</t>
+        </is>
+      </c>
+      <c r="N96" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P96" t="inlineStr">
+        <is>
+          <t>PR</t>
+        </is>
+      </c>
+      <c r="Q96" t="n">
         <v>120000624922</v>
       </c>
-      <c r="N96" t="inlineStr">
-        <is>
-          <t>PR</t>
+      <c r="R96" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -7024,12 +8944,32 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
-      <c r="M97" t="n">
+      <c r="M97" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
+      <c r="N97" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="P97" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
+      <c r="Q97" t="n">
         <v>120000624923</v>
       </c>
-      <c r="N97" t="inlineStr">
-        <is>
-          <t>DC</t>
+      <c r="R97" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -7092,12 +9032,32 @@
           <t>ENSINO FUNDAMENTAL INCOMPLETO</t>
         </is>
       </c>
-      <c r="M98" t="n">
+      <c r="M98" t="inlineStr">
+        <is>
+          <t>PRTB</t>
+        </is>
+      </c>
+      <c r="N98" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="P98" t="inlineStr">
+        <is>
+          <t>PRTB</t>
+        </is>
+      </c>
+      <c r="Q98" t="n">
         <v>120000624924</v>
       </c>
-      <c r="N98" t="inlineStr">
-        <is>
-          <t>PRTB</t>
+      <c r="R98" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -7160,12 +9120,32 @@
           <t>LÊ E ESCREVE</t>
         </is>
       </c>
-      <c r="M99" t="n">
+      <c r="M99" t="inlineStr">
+        <is>
+          <t>PRTB</t>
+        </is>
+      </c>
+      <c r="N99" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O99" t="inlineStr">
+        <is>
+          <t>LÊ E ESCREVE</t>
+        </is>
+      </c>
+      <c r="P99" t="inlineStr">
+        <is>
+          <t>PRTB</t>
+        </is>
+      </c>
+      <c r="Q99" t="n">
         <v>120000624925</v>
       </c>
-      <c r="N99" t="inlineStr">
-        <is>
-          <t>PRTB</t>
+      <c r="R99" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -7228,12 +9208,32 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
-      <c r="M100" t="n">
+      <c r="M100" t="inlineStr">
+        <is>
+          <t>PRTB</t>
+        </is>
+      </c>
+      <c r="N100" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O100" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="P100" t="inlineStr">
+        <is>
+          <t>PRTB</t>
+        </is>
+      </c>
+      <c r="Q100" t="n">
         <v>120000624926</v>
       </c>
-      <c r="N100" t="inlineStr">
-        <is>
-          <t>PRTB</t>
+      <c r="R100" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -7296,12 +9296,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M101" t="n">
+      <c r="M101" t="inlineStr">
+        <is>
+          <t>PSC</t>
+        </is>
+      </c>
+      <c r="N101" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O101" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P101" t="inlineStr">
+        <is>
+          <t>PSC</t>
+        </is>
+      </c>
+      <c r="Q101" t="n">
         <v>120000624927</v>
       </c>
-      <c r="N101" t="inlineStr">
-        <is>
-          <t>PSC</t>
+      <c r="R101" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -7364,12 +9384,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M102" t="n">
+      <c r="M102" t="inlineStr">
+        <is>
+          <t>PSC</t>
+        </is>
+      </c>
+      <c r="N102" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O102" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P102" t="inlineStr">
+        <is>
+          <t>PSC</t>
+        </is>
+      </c>
+      <c r="Q102" t="n">
         <v>120000624928</v>
       </c>
-      <c r="N102" t="inlineStr">
-        <is>
-          <t>PSC</t>
+      <c r="R102" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -7432,12 +9472,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M103" t="n">
+      <c r="M103" t="inlineStr">
+        <is>
+          <t>PSC</t>
+        </is>
+      </c>
+      <c r="N103" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O103" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P103" t="inlineStr">
+        <is>
+          <t>PSC</t>
+        </is>
+      </c>
+      <c r="Q103" t="n">
         <v>120000624929</v>
       </c>
-      <c r="N103" t="inlineStr">
-        <is>
-          <t>PSC</t>
+      <c r="R103" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -7500,12 +9560,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M104" t="n">
+      <c r="M104" t="inlineStr">
+        <is>
+          <t>PTC</t>
+        </is>
+      </c>
+      <c r="N104" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O104" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P104" t="inlineStr">
+        <is>
+          <t>PTC</t>
+        </is>
+      </c>
+      <c r="Q104" t="n">
         <v>120000624930</v>
       </c>
-      <c r="N104" t="inlineStr">
-        <is>
-          <t>PTC</t>
+      <c r="R104" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -7568,12 +9648,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M105" t="n">
+      <c r="M105" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="N105" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O105" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P105" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="Q105" t="n">
         <v>120000625709</v>
       </c>
-      <c r="N105" t="inlineStr">
-        <is>
-          <t>MDB</t>
+      <c r="R105" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -7636,12 +9736,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M106" t="n">
+      <c r="M106" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="N106" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O106" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P106" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="Q106" t="n">
         <v>120000625710</v>
       </c>
-      <c r="N106" t="inlineStr">
-        <is>
-          <t>MDB</t>
+      <c r="R106" t="inlineStr">
+        <is>
+          <t>INDÍGENA</t>
         </is>
       </c>
     </row>
@@ -7704,12 +9824,32 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
-      <c r="M107" t="n">
+      <c r="M107" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="N107" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O107" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="P107" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="Q107" t="n">
         <v>120000625711</v>
       </c>
-      <c r="N107" t="inlineStr">
-        <is>
-          <t>MDB</t>
+      <c r="R107" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -7772,12 +9912,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M108" t="n">
+      <c r="M108" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="N108" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O108" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P108" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="Q108" t="n">
         <v>120000625712</v>
       </c>
-      <c r="N108" t="inlineStr">
-        <is>
-          <t>MDB</t>
+      <c r="R108" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -7840,12 +10000,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M109" t="n">
+      <c r="M109" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="N109" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O109" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P109" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="Q109" t="n">
         <v>120000625713</v>
       </c>
-      <c r="N109" t="inlineStr">
-        <is>
-          <t>MDB</t>
+      <c r="R109" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -7908,12 +10088,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M110" t="n">
+      <c r="M110" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="N110" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O110" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P110" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="Q110" t="n">
         <v>120000625714</v>
       </c>
-      <c r="N110" t="inlineStr">
-        <is>
-          <t>MDB</t>
+      <c r="R110" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -7976,12 +10176,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M111" t="n">
+      <c r="M111" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="N111" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="O111" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P111" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="Q111" t="n">
         <v>120000625715</v>
       </c>
-      <c r="N111" t="inlineStr">
-        <is>
-          <t>MDB</t>
+      <c r="R111" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -8044,12 +10264,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M112" t="n">
+      <c r="M112" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="N112" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O112" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P112" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="Q112" t="n">
         <v>120000625716</v>
       </c>
-      <c r="N112" t="inlineStr">
-        <is>
-          <t>MDB</t>
+      <c r="R112" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -8112,12 +10352,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M113" t="n">
+      <c r="M113" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="N113" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="O113" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P113" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="Q113" t="n">
         <v>120000625717</v>
       </c>
-      <c r="N113" t="inlineStr">
-        <is>
-          <t>MDB</t>
+      <c r="R113" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -8180,12 +10440,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M114" t="n">
+      <c r="M114" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="N114" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O114" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P114" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="Q114" t="n">
         <v>120000625718</v>
       </c>
-      <c r="N114" t="inlineStr">
-        <is>
-          <t>MDB</t>
+      <c r="R114" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -8248,12 +10528,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M115" t="n">
+      <c r="M115" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="N115" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O115" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P115" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="Q115" t="n">
         <v>120000625719</v>
       </c>
-      <c r="N115" t="inlineStr">
-        <is>
-          <t>MDB</t>
+      <c r="R115" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -8316,12 +10616,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M116" t="n">
+      <c r="M116" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="N116" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O116" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P116" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="Q116" t="n">
         <v>120000625720</v>
       </c>
-      <c r="N116" t="inlineStr">
-        <is>
-          <t>MDB</t>
+      <c r="R116" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -8384,12 +10704,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M117" t="n">
+      <c r="M117" t="inlineStr">
+        <is>
+          <t>PRP</t>
+        </is>
+      </c>
+      <c r="N117" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O117" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P117" t="inlineStr">
+        <is>
+          <t>PRP</t>
+        </is>
+      </c>
+      <c r="Q117" t="n">
         <v>120000625721</v>
       </c>
-      <c r="N117" t="inlineStr">
-        <is>
-          <t>PRP</t>
+      <c r="R117" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -8452,12 +10792,32 @@
           <t>ENSINO FUNDAMENTAL INCOMPLETO</t>
         </is>
       </c>
-      <c r="M118" t="n">
+      <c r="M118" t="inlineStr">
+        <is>
+          <t>PPL</t>
+        </is>
+      </c>
+      <c r="N118" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O118" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="P118" t="inlineStr">
+        <is>
+          <t>PPL</t>
+        </is>
+      </c>
+      <c r="Q118" t="n">
         <v>120000627473</v>
       </c>
-      <c r="N118" t="inlineStr">
-        <is>
-          <t>PPL</t>
+      <c r="R118" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -8520,12 +10880,32 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
-      <c r="M119" t="n">
+      <c r="M119" t="inlineStr">
+        <is>
+          <t>PPL</t>
+        </is>
+      </c>
+      <c r="N119" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O119" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="P119" t="inlineStr">
+        <is>
+          <t>PPL</t>
+        </is>
+      </c>
+      <c r="Q119" t="n">
         <v>120000627474</v>
       </c>
-      <c r="N119" t="inlineStr">
-        <is>
-          <t>PPL</t>
+      <c r="R119" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -8588,12 +10968,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M120" t="n">
+      <c r="M120" t="inlineStr">
+        <is>
+          <t>PPL</t>
+        </is>
+      </c>
+      <c r="N120" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O120" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P120" t="inlineStr">
+        <is>
+          <t>PPL</t>
+        </is>
+      </c>
+      <c r="Q120" t="n">
         <v>120000627475</v>
       </c>
-      <c r="N120" t="inlineStr">
-        <is>
-          <t>PPL</t>
+      <c r="R120" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -8656,12 +11056,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M121" t="n">
+      <c r="M121" t="inlineStr">
+        <is>
+          <t>PSL</t>
+        </is>
+      </c>
+      <c r="N121" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O121" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P121" t="inlineStr">
+        <is>
+          <t>PSL</t>
+        </is>
+      </c>
+      <c r="Q121" t="n">
         <v>120000627756</v>
       </c>
-      <c r="N121" t="inlineStr">
-        <is>
-          <t>PSL</t>
+      <c r="R121" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -8724,12 +11144,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M122" t="n">
+      <c r="M122" t="inlineStr">
+        <is>
+          <t>PSB</t>
+        </is>
+      </c>
+      <c r="N122" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O122" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P122" t="inlineStr">
+        <is>
+          <t>PSB</t>
+        </is>
+      </c>
+      <c r="Q122" t="n">
         <v>120000627790</v>
       </c>
-      <c r="N122" t="inlineStr">
-        <is>
-          <t>PSB</t>
+      <c r="R122" t="inlineStr">
+        <is>
+          <t>PRETA</t>
         </is>
       </c>
     </row>
@@ -8792,12 +11232,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M123" t="n">
+      <c r="M123" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="N123" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O123" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P123" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="Q123" t="n">
         <v>120000627877</v>
       </c>
-      <c r="N123" t="inlineStr">
-        <is>
-          <t>MDB</t>
+      <c r="R123" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -8860,12 +11320,32 @@
           <t>ENSINO FUNDAMENTAL COMPLETO</t>
         </is>
       </c>
-      <c r="M124" t="n">
+      <c r="M124" t="inlineStr">
+        <is>
+          <t>PC do B</t>
+        </is>
+      </c>
+      <c r="N124" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O124" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL COMPLETO</t>
+        </is>
+      </c>
+      <c r="P124" t="inlineStr">
+        <is>
+          <t>PC do B</t>
+        </is>
+      </c>
+      <c r="Q124" t="n">
         <v>120000628256</v>
       </c>
-      <c r="N124" t="inlineStr">
-        <is>
-          <t>PC do B</t>
+      <c r="R124" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -8928,12 +11408,32 @@
           <t>ENSINO FUNDAMENTAL COMPLETO</t>
         </is>
       </c>
-      <c r="M125" t="n">
+      <c r="M125" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
+      <c r="N125" t="inlineStr">
+        <is>
+          <t>VIÚVO(A)</t>
+        </is>
+      </c>
+      <c r="O125" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL COMPLETO</t>
+        </is>
+      </c>
+      <c r="P125" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
+      <c r="Q125" t="n">
         <v>120000629021</v>
       </c>
-      <c r="N125" t="inlineStr">
-        <is>
-          <t>PV</t>
+      <c r="R125" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -8996,12 +11496,32 @@
           <t>ENSINO FUNDAMENTAL COMPLETO</t>
         </is>
       </c>
-      <c r="M126" t="n">
+      <c r="M126" t="inlineStr">
+        <is>
+          <t>PPS</t>
+        </is>
+      </c>
+      <c r="N126" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="O126" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL COMPLETO</t>
+        </is>
+      </c>
+      <c r="P126" t="inlineStr">
+        <is>
+          <t>PPS</t>
+        </is>
+      </c>
+      <c r="Q126" t="n">
         <v>120000629493</v>
       </c>
-      <c r="N126" t="inlineStr">
-        <is>
-          <t>PPS</t>
+      <c r="R126" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -9064,12 +11584,32 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
-      <c r="M127" t="n">
+      <c r="M127" t="inlineStr">
+        <is>
+          <t>PRP</t>
+        </is>
+      </c>
+      <c r="N127" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O127" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="P127" t="inlineStr">
+        <is>
+          <t>PRP</t>
+        </is>
+      </c>
+      <c r="Q127" t="n">
         <v>120000629522</v>
       </c>
-      <c r="N127" t="inlineStr">
-        <is>
-          <t>PRP</t>
+      <c r="R127" t="inlineStr">
+        <is>
+          <t>PARDA</t>
         </is>
       </c>
     </row>
@@ -9132,12 +11672,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M128" t="n">
+      <c r="M128" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="N128" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O128" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P128" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="Q128" t="n">
         <v>120000629553</v>
       </c>
-      <c r="N128" t="inlineStr">
-        <is>
-          <t>MDB</t>
+      <c r="R128" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -9200,12 +11760,32 @@
           <t>LÊ E ESCREVE</t>
         </is>
       </c>
-      <c r="M129" t="n">
+      <c r="M129" t="inlineStr">
+        <is>
+          <t>PODE</t>
+        </is>
+      </c>
+      <c r="N129" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O129" t="inlineStr">
+        <is>
+          <t>LÊ E ESCREVE</t>
+        </is>
+      </c>
+      <c r="P129" t="inlineStr">
+        <is>
+          <t>PODE</t>
+        </is>
+      </c>
+      <c r="Q129" t="n">
         <v>120000629760</v>
       </c>
-      <c r="N129" t="inlineStr">
-        <is>
-          <t>PODE</t>
+      <c r="R129" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -9268,12 +11848,32 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
-      <c r="M130" t="n">
+      <c r="M130" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
+      <c r="N130" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O130" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="P130" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
+      <c r="Q130" t="n">
         <v>120000629772</v>
       </c>
-      <c r="N130" t="inlineStr">
-        <is>
-          <t>PV</t>
+      <c r="R130" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>
@@ -9336,12 +11936,32 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
-      <c r="M131" t="n">
+      <c r="M131" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="N131" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="O131" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="P131" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
+      <c r="Q131" t="n">
         <v>120000630102</v>
       </c>
-      <c r="N131" t="inlineStr">
-        <is>
-          <t>MDB</t>
+      <c r="R131" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
         </is>
       </c>
     </row>

</xml_diff>